<commit_message>
* change input of HOUR(), MINUTE(), and VALUE() * STDEVP is not implemented * change orders of methods
</commit_message>
<xml_diff>
--- a/zss.test/src/test/java/org/zkoss/zss/api/impl/book/264-text-formula.xlsx
+++ b/zss.test/src/test/java/org/zkoss/zss/api/impl/book/264-text-formula.xlsx
@@ -384,6 +384,72 @@
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
     <mruColors>
       <color rgb="FF0000FF"/>
       <color rgb="FF3333FF"/>
@@ -402,7 +468,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="C7EDCC"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -681,8 +747,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D224"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A74" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A75" sqref="A75"/>
+    <sheetView tabSelected="1" topLeftCell="A59" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B74" sqref="B74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1378,8 +1444,8 @@
         <v>59</v>
       </c>
       <c r="B73">
-        <f>VALUE("16:48:00")</f>
-        <v>0.70000000000000007</v>
+        <f>VALUE("0.7")</f>
+        <v>0.7</v>
       </c>
       <c r="C73">
         <v>0.7</v>

</xml_diff>